<commit_message>
This is my updated code for Friday Project 10.
</commit_message>
<xml_diff>
--- a/reviews_with_sentiment.xlsx
+++ b/reviews_with_sentiment.xlsx
@@ -465,11 +465,11 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.01666666666666667</v>
+        <v>-0.09899030109339679</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.3</v>
+        <v>0.6475516089082036</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -501,11 +501,11 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.01458333333333334</v>
+        <v>0.04413380580529414</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3020833333333334</v>
+        <v>0.749322346792024</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.04999999999999999</v>
+        <v>-0.6233702274888613</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -555,11 +555,11 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3375</v>
+        <v>0.000878953486077666</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3257142857142857</v>
+        <v>0.2786825308053305</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -591,11 +591,11 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.125</v>
+        <v>-0.3931367970387509</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -609,11 +609,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.75</v>
+        <v>-0.05260177637738402</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.08333333333333333</v>
+        <v>-0.406133221668862</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -645,11 +645,11 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5388888888888889</v>
+        <v>0.00693790114760473</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.225</v>
+        <v>-0.4891867060569277</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -681,11 +681,11 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.2465909090909091</v>
+        <v>0.01484952414969645</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -699,11 +699,11 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6333333333333333</v>
+        <v>0.01156747152330598</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -717,11 +717,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.2</v>
+        <v>-0.5193943617369797</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -735,11 +735,11 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.1777777777777778</v>
+        <v>0.08611197800163442</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -753,11 +753,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.4</v>
+        <v>-0.05612078416268695</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.2761904761904762</v>
+        <v>0.3795056309923407</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -789,11 +789,11 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.2</v>
+        <v>-0.4567682922686051</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.1333333333333333</v>
+        <v>-0.7215454167070601</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -825,11 +825,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.465</v>
+        <v>-0.704367386330657</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -843,11 +843,11 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.2295238095238095</v>
+        <v>0.05009646864856881</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.06944444444444443</v>
+        <v>-0.08982086458710262</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -879,11 +879,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2803571428571429</v>
+        <v>-0.2431844924257217</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5</v>
+        <v>0.2330800645891585</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -915,11 +915,11 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.09999999999999998</v>
+        <v>0.08417874335569822</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -933,11 +933,11 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.5</v>
+        <v>-0.2564881627220614</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.4084125241310997</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -969,11 +969,11 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.2</v>
+        <v>-0.4061499691327267</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.25</v>
+        <v>0.4084053965437379</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1005,11 +1005,11 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.36</v>
+        <v>-0.5122847062040259</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.4702273907451405</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1041,11 +1041,11 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.1</v>
+        <v>0.03896718399218754</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1059,11 +1059,11 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.25</v>
+        <v>-0.6853712231951988</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.05639304090890654</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1095,11 +1095,11 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.3166666666666667</v>
+        <v>-0.6957317975929354</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1113,11 +1113,11 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.5333333333333333</v>
+        <v>-0.2208546591093898</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1131,11 +1131,11 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.75</v>
+        <v>-0.7045125830545405</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1149,11 +1149,11 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.6666666666666666</v>
+        <v>-0.07021213215627867</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.15</v>
+        <v>-0.3188057290312843</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1185,11 +1185,11 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.1333333333333333</v>
+        <v>-0.739159504672815</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1203,11 +1203,11 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>-0.1166666666666667</v>
+        <v>0.4455664616347744</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>-0.2803571428571429</v>
+        <v>-0.7262492821163337</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>-0.15</v>
+        <v>-0.2090776473786516</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1257,11 +1257,11 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>-0.1333333333333333</v>
+        <v>0.03439923790126176</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1275,11 +1275,11 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.125</v>
+        <v>-0.386836377926267</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1293,11 +1293,11 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.475</v>
+        <v>-0.4213442211333231</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1311,11 +1311,11 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>-0.09999999999999999</v>
+        <v>0.04931711468551742</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1329,11 +1329,11 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.2222222222222222</v>
+        <v>-0.3328429135022828</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.0125</v>
+        <v>0.5876963779825463</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>-0.1354166666666667</v>
+        <v>-0.2462190137356823</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1383,11 +1383,11 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.06767676767676767</v>
+        <v>-0.5984289697830769</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1401,11 +1401,11 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.05089285714285714</v>
+        <v>-0.6917715232691061</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1419,11 +1419,11 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>-0.16</v>
+        <v>0.7789985158936701</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>-0.3333333333333333</v>
+        <v>-0.353685057430468</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1455,11 +1455,11 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>0.5750940415225891</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>-0.3166666666666667</v>
+        <v>-0.7263934071703708</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1491,11 +1491,11 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>-0.06249999999999999</v>
+        <v>0.4526293770807616</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -1509,11 +1509,11 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>-0.125</v>
+        <v>0.07803519765759578</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1527,11 +1527,11 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.2916666666666667</v>
+        <v>-0.2043378646821583</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.4916666666666667</v>
+        <v>0.2734978812465426</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1563,11 +1563,11 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.03333333333333333</v>
+        <v>-0.01835985961342608</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1581,11 +1581,11 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.1666666666666667</v>
+        <v>-0.5698911478379212</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>-0.1083333333333333</v>
+        <v>-0.3983527429786172</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1617,11 +1617,11 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.09166666666666667</v>
+        <v>-0.2676184988539407</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1635,11 +1635,11 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.08541666666666665</v>
+        <v>-0.4889929247566807</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1653,11 +1653,11 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.042</v>
+        <v>0.08182282711265823</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1671,11 +1671,11 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>-0.225</v>
+        <v>0.009915583424310356</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1689,11 +1689,11 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.2</v>
+        <v>-0.2883273487265714</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.45</v>
+        <v>0.2427487156843753</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1725,11 +1725,11 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.225</v>
+        <v>0.05553261524814987</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1743,11 +1743,11 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.2</v>
+        <v>-0.4123690346880222</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.669325149101067</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1779,11 +1779,11 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.25</v>
+        <v>-0.07570562440320004</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1797,11 +1797,11 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.1666666666666667</v>
+        <v>-0.4235795808030751</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1815,11 +1815,11 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.2555555555555555</v>
+        <v>-0.03730652901818653</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>0.006285009914272943</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -1851,11 +1851,11 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.2375</v>
+        <v>-0.7782500879418991</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1869,11 +1869,11 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.14375</v>
+        <v>-0.5730518890819443</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -1887,11 +1887,11 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.4166666666666667</v>
+        <v>-0.4587741339993099</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
     </row>

</xml_diff>